<commit_message>
Add new sheets to workbook
</commit_message>
<xml_diff>
--- a/exel_automation/Employees.xlsx
+++ b/exel_automation/Employees.xlsx
@@ -1,45 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\travi\Desktop\Courses\Python Automation\Course Resources\5 - Automating Spreadsheets\7 - Automating Worksheet Operations II - Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BCFFF8-4611-4B1B-ABB1-A508006F1D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Avery Prada" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Junn Patel" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Andrew Dang" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Jen Belosi" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -58,21 +52,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -338,37 +391,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187FF416-6653-4090-8345-E76C288A0440}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6E794C-F1A4-44F5-B140-2C9C5C1F3F4A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add script to delete sheet names matching regex pattern
</commit_message>
<xml_diff>
--- a/exel_automation/Employees.xlsx
+++ b/exel_automation/Employees.xlsx
@@ -6,13 +6,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Avery Prada" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Junn Patel" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Andrew Dang" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Jen Belosi" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Avery Prada" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Junn Patel" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Andrew Dang" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Jen Belosi" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -402,9 +399,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -420,9 +417,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -434,13 +431,13 @@
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -460,58 +457,4 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>